<commit_message>
create testcase for login unsuccessfully with email that haven't already existed
</commit_message>
<xml_diff>
--- a/DataObjects/InvalidPassword.xlsx
+++ b/DataObjects/InvalidPassword.xlsx
@@ -31,10 +31,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -57,16 +65,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -366,39 +379,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="39.140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1234567</v>
       </c>
+      <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>